<commit_message>
new branch for C/S interfaces implementation
</commit_message>
<xml_diff>
--- a/Import/Application.xlsx
+++ b/Import/Application.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771E2174-7BA9-4BCC-8A01-158D60DE7B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA546488-1807-4241-BDBB-2DD8BC6DC53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="169">
   <si>
     <t>TypeName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,10 +76,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>e_UsageMode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Value Table</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -121,10 +117,6 @@
   </si>
   <si>
     <t>BatteryMode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>e_BatteryMode</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -394,6 +386,322 @@
   </si>
   <si>
     <t>SWC1, Delegation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CockpitService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C/S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operations</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arguments</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetAmbientTemp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetInteriorTemp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReturnValueType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_NOT_OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SetHvacCtrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACCTR_ACCEPT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACCTR_PARAMERROR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACCTR_MODEERROR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnOff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OperationMode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CirculationMode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FanCtrMode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TargetTemp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReturnCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ArgsType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alias</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reference Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scaling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Offset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>℃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sint16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Km/h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_BatteryMode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_UsageMode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_Temperature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_VehicleSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_StdReturn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_HvacCtrReturn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>signed short</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_HvacOnOff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACSW_NONE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACSW_ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACSW_0FF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_HvacOperationMode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_HvacCirculationMode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACCIRC_NONE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACOP_NONE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACOP_DEMIST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACOP_HEAT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACOP_REFRIG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACOP_AUTO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACCIRC_INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACCIRC_EXT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_HvacFanCtrMode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACFANCTR_NONE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACFANCTR_FACE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACFANCTR_UP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_HVACFANCTR_DOWN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MotorCtrService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_MotorCtrCmd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_MOTORCTRCMD_NONE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_MOTORCTRCMD_OPEN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_MOTORCTRCMD_CLOSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cmd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_MotorCtrErr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_MOTORCTRERR_ACCEPT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_MOTORCTRERR_DENIED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lastStopReason</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MotorRunning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INOUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveRequest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DoorLockService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LockRequest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetDoorStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LookUpDoorCfg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IndexResult</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ErrCode</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -453,7 +761,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -735,13 +1043,108 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -865,10 +1268,49 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1185,25 +1627,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A675E1F-9C03-4EE3-AE97-C268A8F23FBE}">
-  <dimension ref="B1:E31"/>
+  <dimension ref="B1:I71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.125" customWidth="1"/>
-    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="2" max="2" width="21.375" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="21.875" customWidth="1"/>
-    <col min="5" max="5" width="19.25" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="8" max="9" width="9" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="7" max="7" width="13.125" customWidth="1"/>
+    <col min="8" max="8" width="12.125" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
@@ -1211,19 +1655,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
@@ -1237,7 +1681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
@@ -1251,7 +1695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
         <v>9</v>
       </c>
@@ -1265,9 +1709,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>4</v>
@@ -1276,228 +1720,671 @@
         <v>32</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-    </row>
-    <row r="9" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B8" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="48">
+        <v>16</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C11" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D11" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="I11" s="29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B13" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="16">
+        <v>-40</v>
+      </c>
+      <c r="G13" s="16">
+        <v>-80</v>
+      </c>
+      <c r="H13" s="16">
+        <v>120</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B14" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="37">
+        <v>5.6250000000000001E-2</v>
+      </c>
+      <c r="F14" s="37">
+        <v>0</v>
+      </c>
+      <c r="G14" s="37">
+        <v>0</v>
+      </c>
+      <c r="H14" s="37">
+        <v>240</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+    </row>
+    <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B19" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="17">
+      <c r="E19" s="17">
         <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="20"/>
-    </row>
-    <row r="18" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="17">
-        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
       <c r="D20" s="24" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E20" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="11"/>
-    </row>
-    <row r="23" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="1"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B23" s="15"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="20"/>
     </row>
     <row r="25" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B25" s="15" t="s">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
-      <c r="D26" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>2</v>
+      <c r="D26" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
-      <c r="D27" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="17" t="s">
+      <c r="D27" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="20"/>
     </row>
     <row r="29" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B30" s="30"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B31" s="18"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="20"/>
+    </row>
+    <row r="32" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B32" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B33" s="30"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B34" s="30"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B35" s="18"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="20"/>
+    </row>
+    <row r="36" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B36" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="E36" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B37" s="30"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B38" s="30"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="E38" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B39" s="18"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="20"/>
+    </row>
+    <row r="40" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B40" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B41" s="30"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="E41" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B42" s="30"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="E42" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B43" s="30"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="E43" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B44" s="30"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E44" s="38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B45" s="18"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="20"/>
+    </row>
+    <row r="46" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B46" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B47" s="30"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="E47" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B48" s="30"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="E48" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B49" s="18"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="20"/>
+    </row>
+    <row r="50" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B50" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="C50" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="E50" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B51" s="30"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B52" s="30"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B53" s="30"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B54" s="18"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="20"/>
+    </row>
+    <row r="55" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B55" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="E55" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B56" s="30"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B57" s="30"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E57" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B58" s="18"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="20"/>
+    </row>
+    <row r="59" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B59" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="E59" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B60" s="30"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="E60" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="7"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="9"/>
+    </row>
+    <row r="62" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D62" s="11"/>
+    </row>
+    <row r="63" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B64" s="1"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B65" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B66" s="15"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B67" s="15"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B68" s="18"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="20"/>
+    </row>
+    <row r="69" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B69" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="16" t="s">
+      <c r="E69" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B70" s="15"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B30" s="15"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="9"/>
+      <c r="E70" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="7"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1508,10 +2395,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA44D0C-18C8-469C-9219-A37B0C48C99E}">
-  <dimension ref="B2:E15"/>
+  <dimension ref="B2:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1520,141 +2407,509 @@
     <col min="2" max="2" width="22.5" customWidth="1"/>
     <col min="3" max="3" width="16.25" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="17.25" customWidth="1"/>
+    <col min="7" max="7" width="22.75" customWidth="1"/>
+    <col min="8" max="8" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="36" t="s">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="D3" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
+    </row>
+    <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>82</v>
+        <v>37</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
-      <c r="C6" s="32"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
-      <c r="C7" s="32"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>36</v>
-      </c>
       <c r="E9" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
-      <c r="C10" s="32"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="18"/>
-      <c r="C11" s="41"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>82</v>
+        <v>33</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="26"/>
-    </row>
-    <row r="14" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="55"/>
+    </row>
+    <row r="14" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B14" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
-      <c r="C15" s="35"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="26"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B18" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="H18" s="45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B20" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B23" s="15"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B24" s="15"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B25" s="15"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B26" s="15"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
+    </row>
+    <row r="29" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B29" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="20"/>
+    </row>
+    <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B34" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B35" s="15"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B36" s="15"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B37" s="15"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B38" s="30"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="G38" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="21"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1667,7 +2922,7 @@
   <dimension ref="B1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1686,31 +2941,31 @@
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
@@ -1726,21 +2981,21 @@
     </row>
     <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I4" s="16"/>
       <c r="J4" s="17"/>
@@ -1749,17 +3004,17 @@
       <c r="B5" s="15"/>
       <c r="C5" s="32"/>
       <c r="D5" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="17"/>
@@ -1768,63 +3023,63 @@
       <c r="B6" s="15"/>
       <c r="C6" s="32"/>
       <c r="D6" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
       <c r="C7" s="32"/>
       <c r="D7" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
       <c r="C8" s="32"/>
       <c r="D8" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -1840,21 +3095,21 @@
     </row>
     <row r="10" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="17"/>
@@ -1863,17 +3118,17 @@
       <c r="B11" s="15"/>
       <c r="C11" s="32"/>
       <c r="D11" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
@@ -1882,21 +3137,21 @@
       <c r="B12" s="15"/>
       <c r="C12" s="32"/>
       <c r="D12" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
@@ -1912,69 +3167,69 @@
     </row>
     <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>71</v>
-      </c>
       <c r="F14" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
       <c r="C15" s="32"/>
       <c r="D15" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
       <c r="C16" s="32"/>
       <c r="D16" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
       <c r="I16" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="J16" s="42" t="s">
-        <v>84</v>
+        <v>72</v>
+      </c>
+      <c r="J16" s="41" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
@@ -1990,45 +3245,45 @@
     </row>
     <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B18" s="39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B19" s="30"/>
       <c r="C19" s="34"/>
       <c r="D19" s="37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G19" s="37"/>
       <c r="H19" s="37"/>
       <c r="I19" s="37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J19" s="38"/>
     </row>

</xml_diff>

<commit_message>
get alias type form import
</commit_message>
<xml_diff>
--- a/Import/Application.xlsx
+++ b/Import/Application.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\Import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\ArxmlTools\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA546488-1807-4241-BDBB-2DD8BC6DC53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB597416-A5D5-44E9-9A9F-59B0B82FEAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25840" windowHeight="14027" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTypes" sheetId="1" r:id="rId1"/>
@@ -497,10 +497,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Min Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MaxValue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -702,6 +698,10 @@
   </si>
   <si>
     <t>ErrCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MinValue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1629,25 +1629,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A675E1F-9C03-4EE3-AE97-C268A8F23FBE}">
   <dimension ref="B1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.7" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.125" customWidth="1"/>
-    <col min="2" max="2" width="21.375" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="24.5" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="14.75" customWidth="1"/>
-    <col min="7" max="7" width="13.125" customWidth="1"/>
-    <col min="8" max="8" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="15.35" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="20.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
@@ -1661,13 +1661,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>9</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>77</v>
       </c>
@@ -1723,9 +1723,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" s="37" t="s">
         <v>4</v>
@@ -1734,17 +1734,17 @@
         <v>16</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="21"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="23"/>
     </row>
-    <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="15.35" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:9" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="27" t="s">
         <v>0</v>
       </c>
@@ -1761,16 +1761,16 @@
         <v>116</v>
       </c>
       <c r="G11" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="H11" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="I11" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="I11" s="29" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -1780,15 +1780,15 @@
       <c r="H12" s="13"/>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>113</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E13" s="16">
         <v>0.1</v>
@@ -1803,18 +1803,18 @@
         <v>120</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C14" s="37" t="s">
         <v>113</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E14" s="37">
         <v>5.6250000000000001E-2</v>
@@ -1829,10 +1829,10 @@
         <v>240</v>
       </c>
       <c r="I14" s="38" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -1842,8 +1842,8 @@
       <c r="H15" s="22"/>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="15.35" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:5" ht="20.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="27" t="s">
         <v>0</v>
       </c>
@@ -1857,15 +1857,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>11</v>
@@ -1877,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
       <c r="D20" s="24" t="s">
@@ -1887,7 +1887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
       <c r="D21" s="24" t="s">
@@ -1897,7 +1897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
       <c r="D22" s="24" t="s">
@@ -1907,7 +1907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
       <c r="D23" s="24" t="s">
@@ -1917,15 +1917,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
       <c r="D24" s="25"/>
       <c r="E24" s="20"/>
     </row>
-    <row r="25" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>11</v>
@@ -1937,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
       <c r="D26" s="24" t="s">
@@ -1947,7 +1947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
       <c r="D27" s="24" t="s">
@@ -1957,15 +1957,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
       <c r="D28" s="25"/>
       <c r="E28" s="20"/>
     </row>
-    <row r="29" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C29" s="37" t="s">
         <v>11</v>
@@ -1977,7 +1977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="30"/>
       <c r="C30" s="37"/>
       <c r="D30" s="42" t="s">
@@ -1987,15 +1987,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
       <c r="C31" s="19"/>
       <c r="D31" s="25"/>
       <c r="E31" s="20"/>
     </row>
-    <row r="32" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C32" s="37" t="s">
         <v>11</v>
@@ -2007,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="30"/>
       <c r="C33" s="37"/>
       <c r="D33" s="42" t="s">
@@ -2017,7 +2017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="30"/>
       <c r="C34" s="37"/>
       <c r="D34" s="42" t="s">
@@ -2027,276 +2027,276 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="18"/>
       <c r="C35" s="19"/>
       <c r="D35" s="25"/>
       <c r="E35" s="20"/>
     </row>
-    <row r="36" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E36" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="30"/>
       <c r="C37" s="37"/>
       <c r="D37" s="42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E37" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="30"/>
       <c r="C38" s="37"/>
       <c r="D38" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E38" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="18"/>
       <c r="C39" s="19"/>
       <c r="D39" s="25"/>
       <c r="E39" s="20"/>
     </row>
-    <row r="40" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C40" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E40" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="30"/>
       <c r="C41" s="37"/>
       <c r="D41" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E41" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="30"/>
       <c r="C42" s="37"/>
       <c r="D42" s="42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E42" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="30"/>
       <c r="C43" s="37"/>
       <c r="D43" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E43" s="38">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="30"/>
       <c r="C44" s="37"/>
       <c r="D44" s="42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E44" s="38">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="18"/>
       <c r="C45" s="19"/>
       <c r="D45" s="25"/>
       <c r="E45" s="20"/>
     </row>
-    <row r="46" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C46" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E46" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="30"/>
       <c r="C47" s="37"/>
       <c r="D47" s="42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E47" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="30"/>
       <c r="C48" s="37"/>
       <c r="D48" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E48" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="18"/>
       <c r="C49" s="19"/>
       <c r="D49" s="25"/>
       <c r="E49" s="20"/>
     </row>
-    <row r="50" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C50" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D50" s="42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E50" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="30"/>
       <c r="C51" s="37"/>
       <c r="D51" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E51" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="30"/>
       <c r="C52" s="37"/>
       <c r="D52" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E52" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="30"/>
       <c r="C53" s="37"/>
       <c r="D53" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E53" s="38">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="18"/>
       <c r="C54" s="19"/>
       <c r="D54" s="25"/>
       <c r="E54" s="20"/>
     </row>
-    <row r="55" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C55" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D55" s="42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E55" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="30"/>
       <c r="C56" s="37"/>
       <c r="D56" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E56" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="30"/>
       <c r="C57" s="37"/>
       <c r="D57" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E57" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="18"/>
       <c r="C58" s="19"/>
       <c r="D58" s="25"/>
       <c r="E58" s="20"/>
     </row>
-    <row r="59" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C59" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D59" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E59" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="30"/>
       <c r="C60" s="37"/>
       <c r="D60" s="42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E60" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
       <c r="D61" s="10"/>
       <c r="E61" s="9"/>
     </row>
-    <row r="62" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D62" s="11"/>
     </row>
-    <row r="63" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" ht="20.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="27" t="s">
         <v>0</v>
       </c>
@@ -2310,13 +2310,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="15" t="s">
         <v>15</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="15"/>
       <c r="C66" s="16"/>
       <c r="D66" s="16" t="s">
@@ -2340,7 +2340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="15"/>
       <c r="C67" s="16"/>
       <c r="D67" s="16" t="s">
@@ -2350,13 +2350,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="18"/>
       <c r="C68" s="19"/>
       <c r="D68" s="19"/>
       <c r="E68" s="20"/>
     </row>
-    <row r="69" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="15" t="s">
         <v>20</v>
       </c>
@@ -2367,20 +2367,20 @@
         <v>21</v>
       </c>
       <c r="E69" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="15"/>
       <c r="C70" s="16"/>
       <c r="D70" s="16" t="s">
         <v>22</v>
       </c>
       <c r="E70" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
       <c r="D71" s="10"/>
@@ -2397,28 +2397,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA44D0C-18C8-469C-9219-A37B0C48C99E}">
   <dimension ref="B2:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.7" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.125" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="19.5" customWidth="1"/>
-    <col min="6" max="6" width="17.25" customWidth="1"/>
-    <col min="7" max="7" width="22.75" customWidth="1"/>
-    <col min="8" max="8" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="22.77734375" customWidth="1"/>
+    <col min="8" max="8" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="20.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="49" t="s">
         <v>41</v>
       </c>
@@ -2432,13 +2432,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="52"/>
       <c r="C4" s="53"/>
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>37</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16" t="s">
@@ -2462,7 +2462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16" t="s">
@@ -2472,13 +2472,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>32</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16" t="s">
@@ -2502,13 +2502,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>33</v>
       </c>
@@ -2522,13 +2522,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="55"/>
     </row>
-    <row r="14" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>72</v>
       </c>
@@ -2542,14 +2542,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="26"/>
     </row>
-    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="15.35" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="43" t="s">
         <v>41</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -2581,7 +2581,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
         <v>90</v>
       </c>
@@ -2592,57 +2592,57 @@
         <v>94</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>36</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H20" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16" t="s">
         <v>95</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>36</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H21" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16" t="s">
         <v>101</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>105</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H22" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -2651,13 +2651,13 @@
         <v>106</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H23" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
@@ -2666,13 +2666,13 @@
         <v>107</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H24" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
@@ -2681,13 +2681,13 @@
         <v>109</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H25" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -2696,13 +2696,13 @@
         <v>110</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H26" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -2711,13 +2711,13 @@
         <v>111</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -2726,30 +2726,30 @@
       <c r="G28" s="19"/>
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>91</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H29" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="15"/>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
@@ -2758,20 +2758,20 @@
         <v>96</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H30" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="15"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>96</v>
@@ -2783,26 +2783,26 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F32" s="16" t="s">
         <v>159</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>160</v>
       </c>
       <c r="G32" s="16" t="s">
         <v>2</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -2811,21 +2811,21 @@
       <c r="G33" s="19"/>
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>91</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G34" s="16" t="s">
         <v>7</v>
@@ -2834,7 +2834,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="15"/>
       <c r="C35" s="16"/>
       <c r="D35" s="16"/>
@@ -2849,14 +2849,14 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="15"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>96</v>
@@ -2868,32 +2868,32 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="15"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" s="16" t="s">
         <v>166</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>167</v>
       </c>
       <c r="G37" s="16" t="s">
         <v>7</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="30"/>
       <c r="C38" s="37"/>
       <c r="D38" s="37"/>
       <c r="E38" s="37"/>
       <c r="F38" s="37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G38" s="37" t="s">
         <v>7</v>
@@ -2902,7 +2902,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="21"/>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
@@ -2921,25 +2921,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A1755F-5E81-4222-BC5B-9CFC616875A8}">
   <dimension ref="B1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.7" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="5" max="5" width="22.5" customWidth="1"/>
-    <col min="6" max="6" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="15.25" customWidth="1"/>
-    <col min="9" max="9" width="21.5" customWidth="1"/>
-    <col min="10" max="10" width="40.625" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" customWidth="1"/>
+    <col min="10" max="10" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="15.35" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="20.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="27" t="s">
         <v>42</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="31"/>
       <c r="D3" s="2"/>
@@ -2979,7 +2979,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>46</v>
       </c>
@@ -3000,7 +3000,7 @@
       <c r="I4" s="16"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="15"/>
       <c r="C5" s="32"/>
       <c r="D5" s="16" t="s">
@@ -3019,7 +3019,7 @@
       <c r="I5" s="16"/>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="15"/>
       <c r="C6" s="32"/>
       <c r="D6" s="16" t="s">
@@ -3040,7 +3040,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="15"/>
       <c r="C7" s="32"/>
       <c r="D7" s="16" t="s">
@@ -3061,7 +3061,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
       <c r="C8" s="32"/>
       <c r="D8" s="16" t="s">
@@ -3082,7 +3082,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="33"/>
       <c r="D9" s="5"/>
@@ -3093,7 +3093,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>55</v>
       </c>
@@ -3114,7 +3114,7 @@
       <c r="I10" s="16"/>
       <c r="J10" s="17"/>
     </row>
-    <row r="11" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
       <c r="C11" s="32"/>
       <c r="D11" s="16" t="s">
@@ -3133,7 +3133,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="C12" s="32"/>
       <c r="D12" s="16" t="s">
@@ -3154,7 +3154,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="33"/>
       <c r="D13" s="5"/>
@@ -3165,7 +3165,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>66</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="32"/>
       <c r="D15" s="16" t="s">
@@ -3211,7 +3211,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" ht="29.35" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" s="32"/>
       <c r="D16" s="16" t="s">
@@ -3232,7 +3232,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="33"/>
       <c r="D17" s="5"/>
@@ -3243,7 +3243,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="39" t="s">
         <v>83</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="30"/>
       <c r="C19" s="34"/>
       <c r="D19" s="37" t="s">
@@ -3287,7 +3287,7 @@
       </c>
       <c r="J19" s="38"/>
     </row>
-    <row r="20" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="35"/>
       <c r="D20" s="8"/>

</xml_diff>

<commit_message>
add alias datatype implementation
</commit_message>
<xml_diff>
--- a/Import/Application.xlsx
+++ b/Import/Application.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\ArxmlTools\Import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB597416-A5D5-44E9-9A9F-59B0B82FEAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7A115D-CC1D-485A-B309-401D0F0D76F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25840" windowHeight="14027" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTypes" sheetId="1" r:id="rId1"/>
@@ -505,18 +505,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>℃</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sint16</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Km/h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>t_BatteryMode</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -702,6 +694,14 @@
   </si>
   <si>
     <t>MinValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kmperh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DegreeC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1630,24 +1630,24 @@
   <dimension ref="B1:I71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.7" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.125" customWidth="1"/>
+    <col min="2" max="2" width="21.375" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="7" max="7" width="13.125" customWidth="1"/>
+    <col min="8" max="8" width="12.125" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.35" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="20.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
@@ -1661,13 +1661,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
         <v>9</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="15" t="s">
         <v>77</v>
       </c>
@@ -1723,9 +1723,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="37" t="s">
         <v>4</v>
@@ -1734,17 +1734,17 @@
         <v>16</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="23"/>
     </row>
-    <row r="10" spans="2:9" ht="15.35" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="2:9" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
         <v>0</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>116</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>117</v>
@@ -1770,7 +1770,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -1780,15 +1780,15 @@
       <c r="H12" s="13"/>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>113</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E13" s="16">
         <v>0.1</v>
@@ -1803,18 +1803,18 @@
         <v>120</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C14" s="37" t="s">
         <v>113</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E14" s="37">
         <v>5.6250000000000001E-2</v>
@@ -1829,10 +1829,10 @@
         <v>240</v>
       </c>
       <c r="I14" s="38" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -1842,8 +1842,8 @@
       <c r="H15" s="22"/>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" spans="2:9" ht="15.35" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:5" ht="20.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="27" t="s">
         <v>0</v>
       </c>
@@ -1857,15 +1857,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B19" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>11</v>
@@ -1877,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
       <c r="D20" s="24" t="s">
@@ -1887,7 +1887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
       <c r="D21" s="24" t="s">
@@ -1897,7 +1897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
       <c r="D22" s="24" t="s">
@@ -1907,7 +1907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
       <c r="D23" s="24" t="s">
@@ -1917,15 +1917,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
       <c r="D24" s="25"/>
       <c r="E24" s="20"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B25" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>11</v>
@@ -1937,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
       <c r="D26" s="24" t="s">
@@ -1947,7 +1947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
       <c r="D27" s="24" t="s">
@@ -1957,15 +1957,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
       <c r="D28" s="25"/>
       <c r="E28" s="20"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B29" s="30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C29" s="37" t="s">
         <v>11</v>
@@ -1977,7 +1977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B30" s="30"/>
       <c r="C30" s="37"/>
       <c r="D30" s="42" t="s">
@@ -1987,15 +1987,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B31" s="18"/>
       <c r="C31" s="19"/>
       <c r="D31" s="25"/>
       <c r="E31" s="20"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B32" s="30" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C32" s="37" t="s">
         <v>11</v>
@@ -2007,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B33" s="30"/>
       <c r="C33" s="37"/>
       <c r="D33" s="42" t="s">
@@ -2017,7 +2017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B34" s="30"/>
       <c r="C34" s="37"/>
       <c r="D34" s="42" t="s">
@@ -2027,276 +2027,276 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="19"/>
       <c r="D35" s="25"/>
       <c r="E35" s="20"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B36" s="30" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C36" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E36" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B37" s="30"/>
       <c r="C37" s="37"/>
       <c r="D37" s="42" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E37" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B38" s="30"/>
       <c r="C38" s="37"/>
       <c r="D38" s="42" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E38" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B39" s="18"/>
       <c r="C39" s="19"/>
       <c r="D39" s="25"/>
       <c r="E39" s="20"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B40" s="30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C40" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="42" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E40" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B41" s="30"/>
       <c r="C41" s="37"/>
       <c r="D41" s="42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E41" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B42" s="30"/>
       <c r="C42" s="37"/>
       <c r="D42" s="42" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E42" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B43" s="30"/>
       <c r="C43" s="37"/>
       <c r="D43" s="42" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E43" s="38">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B44" s="30"/>
       <c r="C44" s="37"/>
       <c r="D44" s="42" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E44" s="38">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B45" s="18"/>
       <c r="C45" s="19"/>
       <c r="D45" s="25"/>
       <c r="E45" s="20"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B46" s="30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C46" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E46" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B47" s="30"/>
       <c r="C47" s="37"/>
       <c r="D47" s="42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E47" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B48" s="30"/>
       <c r="C48" s="37"/>
       <c r="D48" s="42" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E48" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B49" s="18"/>
       <c r="C49" s="19"/>
       <c r="D49" s="25"/>
       <c r="E49" s="20"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B50" s="30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C50" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D50" s="42" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E50" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B51" s="30"/>
       <c r="C51" s="37"/>
       <c r="D51" s="42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E51" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B52" s="30"/>
       <c r="C52" s="37"/>
       <c r="D52" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E52" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B53" s="30"/>
       <c r="C53" s="37"/>
       <c r="D53" s="42" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E53" s="38">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B54" s="18"/>
       <c r="C54" s="19"/>
       <c r="D54" s="25"/>
       <c r="E54" s="20"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B55" s="30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C55" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D55" s="42" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E55" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B56" s="30"/>
       <c r="C56" s="37"/>
       <c r="D56" s="42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E56" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B57" s="30"/>
       <c r="C57" s="37"/>
       <c r="D57" s="42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E57" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B58" s="18"/>
       <c r="C58" s="19"/>
       <c r="D58" s="25"/>
       <c r="E58" s="20"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B59" s="30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C59" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D59" s="42" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E59" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B60" s="30"/>
       <c r="C60" s="37"/>
       <c r="D60" s="42" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E60" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:5" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
       <c r="D61" s="10"/>
       <c r="E61" s="9"/>
     </row>
-    <row r="62" spans="2:5" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D62" s="11"/>
     </row>
-    <row r="63" spans="2:5" ht="20.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B63" s="27" t="s">
         <v>0</v>
       </c>
@@ -2310,13 +2310,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="1"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B65" s="15" t="s">
         <v>15</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B66" s="15"/>
       <c r="C66" s="16"/>
       <c r="D66" s="16" t="s">
@@ -2340,7 +2340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B67" s="15"/>
       <c r="C67" s="16"/>
       <c r="D67" s="16" t="s">
@@ -2350,13 +2350,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B68" s="18"/>
       <c r="C68" s="19"/>
       <c r="D68" s="19"/>
       <c r="E68" s="20"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B69" s="15" t="s">
         <v>20</v>
       </c>
@@ -2367,20 +2367,20 @@
         <v>21</v>
       </c>
       <c r="E69" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B70" s="15"/>
       <c r="C70" s="16"/>
       <c r="D70" s="16" t="s">
         <v>22</v>
       </c>
       <c r="E70" s="17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
       <c r="D71" s="10"/>
@@ -2401,24 +2401,24 @@
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.7" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.109375" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="1" max="1" width="6.125" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="16.25" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" customWidth="1"/>
-    <col min="7" max="7" width="22.77734375" customWidth="1"/>
-    <col min="8" max="8" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="17.25" customWidth="1"/>
+    <col min="7" max="7" width="22.75" customWidth="1"/>
+    <col min="8" max="8" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="2:8" ht="20.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="49" t="s">
         <v>41</v>
       </c>
@@ -2432,13 +2432,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="52"/>
       <c r="C4" s="53"/>
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
         <v>37</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16" t="s">
@@ -2462,7 +2462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16" t="s">
@@ -2472,13 +2472,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
         <v>32</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16" t="s">
@@ -2502,13 +2502,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="15" t="s">
         <v>33</v>
       </c>
@@ -2522,13 +2522,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="55"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="15" t="s">
         <v>72</v>
       </c>
@@ -2542,14 +2542,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="26"/>
     </row>
-    <row r="17" spans="2:8" ht="15.35" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B18" s="43" t="s">
         <v>41</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -2581,7 +2581,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B20" s="15" t="s">
         <v>90</v>
       </c>
@@ -2592,57 +2592,57 @@
         <v>94</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>36</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H20" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16" t="s">
         <v>95</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>36</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H21" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16" t="s">
         <v>101</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>105</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H22" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -2651,13 +2651,13 @@
         <v>106</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H23" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
@@ -2666,13 +2666,13 @@
         <v>107</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H24" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
@@ -2681,13 +2681,13 @@
         <v>109</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H25" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -2696,13 +2696,13 @@
         <v>110</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H26" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -2711,13 +2711,13 @@
         <v>111</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -2726,30 +2726,30 @@
       <c r="G28" s="19"/>
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B29" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>91</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H29" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B30" s="15"/>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
@@ -2758,20 +2758,20 @@
         <v>96</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H30" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B31" s="15"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>96</v>
@@ -2783,26 +2783,26 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G32" s="16" t="s">
         <v>2</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -2811,21 +2811,21 @@
       <c r="G33" s="19"/>
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B34" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>91</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G34" s="16" t="s">
         <v>7</v>
@@ -2834,7 +2834,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B35" s="15"/>
       <c r="C35" s="16"/>
       <c r="D35" s="16"/>
@@ -2849,14 +2849,14 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B36" s="15"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>96</v>
@@ -2868,32 +2868,32 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B37" s="15"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G37" s="16" t="s">
         <v>7</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B38" s="30"/>
       <c r="C38" s="37"/>
       <c r="D38" s="37"/>
       <c r="E38" s="37"/>
       <c r="F38" s="37" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G38" s="37" t="s">
         <v>7</v>
@@ -2902,7 +2902,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="21"/>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
@@ -2925,21 +2925,21 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.7" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="11.875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" customWidth="1"/>
-    <col min="10" max="10" width="40.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.25" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="10" max="10" width="40.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.35" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="20.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
         <v>42</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="31"/>
       <c r="D3" s="2"/>
@@ -2979,7 +2979,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="15" t="s">
         <v>46</v>
       </c>
@@ -3000,7 +3000,7 @@
       <c r="I4" s="16"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
       <c r="C5" s="32"/>
       <c r="D5" s="16" t="s">
@@ -3019,7 +3019,7 @@
       <c r="I5" s="16"/>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
       <c r="C6" s="32"/>
       <c r="D6" s="16" t="s">
@@ -3040,7 +3040,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
       <c r="C7" s="32"/>
       <c r="D7" s="16" t="s">
@@ -3061,7 +3061,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
       <c r="C8" s="32"/>
       <c r="D8" s="16" t="s">
@@ -3082,7 +3082,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
       <c r="C9" s="33"/>
       <c r="D9" s="5"/>
@@ -3093,7 +3093,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
         <v>55</v>
       </c>
@@ -3114,7 +3114,7 @@
       <c r="I10" s="16"/>
       <c r="J10" s="17"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
       <c r="C11" s="32"/>
       <c r="D11" s="16" t="s">
@@ -3133,7 +3133,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
       <c r="C12" s="32"/>
       <c r="D12" s="16" t="s">
@@ -3154,7 +3154,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
       <c r="C13" s="33"/>
       <c r="D13" s="5"/>
@@ -3165,7 +3165,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="15" t="s">
         <v>66</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
       <c r="C15" s="32"/>
       <c r="D15" s="16" t="s">
@@ -3211,7 +3211,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="29.35" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
       <c r="C16" s="32"/>
       <c r="D16" s="16" t="s">
@@ -3232,7 +3232,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="4"/>
       <c r="C17" s="33"/>
       <c r="D17" s="5"/>
@@ -3243,7 +3243,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B18" s="39" t="s">
         <v>83</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B19" s="30"/>
       <c r="C19" s="34"/>
       <c r="D19" s="37" t="s">
@@ -3287,7 +3287,7 @@
       </c>
       <c r="J19" s="38"/>
     </row>
-    <row r="20" spans="2:10" ht="15.35" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="35"/>
       <c r="D20" s="8"/>

</xml_diff>

<commit_message>
add cs port interfaces extract method
</commit_message>
<xml_diff>
--- a/Import/Application.xlsx
+++ b/Import/Application.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7A115D-CC1D-485A-B309-401D0F0D76F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBC1F4E-445B-4FC5-A91B-EC244468CC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTypes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="170">
   <si>
     <t>TypeName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -702,6 +702,10 @@
   </si>
   <si>
     <t>DegreeC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RefreshRequest</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1144,7 +1148,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1273,15 +1277,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1629,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A675E1F-9C03-4EE3-AE97-C268A8F23FBE}">
   <dimension ref="B1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1730,7 +1725,7 @@
       <c r="C8" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D8" s="45">
         <v>16</v>
       </c>
       <c r="E8" s="38" t="s">
@@ -1775,7 +1770,7 @@
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="46"/>
+      <c r="F12" s="43"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="14"/>
@@ -1813,7 +1808,7 @@
       <c r="C14" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="45" t="s">
         <v>119</v>
       </c>
       <c r="E14" s="37">
@@ -2395,10 +2390,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA44D0C-18C8-469C-9219-A37B0C48C99E}">
-  <dimension ref="B2:H39"/>
+  <dimension ref="B2:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2419,24 +2414,24 @@
       <c r="H2" s="11"/>
     </row>
     <row r="3" spans="2:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="48" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="52"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="51"/>
     </row>
     <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
@@ -2526,7 +2521,7 @@
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="55"/>
+      <c r="E13" s="52"/>
     </row>
     <row r="14" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="15" t="s">
@@ -2549,37 +2544,37 @@
       <c r="E15" s="26"/>
     </row>
     <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="43" t="s">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="G18" s="44" t="s">
+      <c r="G18" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="H18" s="45" t="s">
+      <c r="H18" s="29" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="20"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B20" s="15" t="s">
@@ -2718,66 +2713,60 @@
       </c>
     </row>
     <row r="28" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="20"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20"/>
+    </row>
+    <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B30" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C30" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D30" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E30" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F30" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="G29" s="16" t="s">
+      <c r="G30" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H30" s="17" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B30" s="15"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B31" s="15"/>
       <c r="C31" s="16"/>
-      <c r="D31" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>124</v>
-      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
       <c r="F31" s="16" t="s">
         <v>96</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>7</v>
+        <v>152</v>
       </c>
       <c r="H31" s="17" t="s">
         <v>97</v>
@@ -2787,77 +2776,77 @@
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E32" s="16" t="s">
         <v>124</v>
       </c>
       <c r="F32" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B33" s="15"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="F33" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="G33" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H33" s="17" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="20"/>
-    </row>
     <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="20"/>
+    </row>
+    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B35" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C35" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D35" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E35" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F35" s="16" t="s">
         <v>151</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B35" s="15"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>7</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B36" s="15"/>
       <c r="C36" s="16"/>
-      <c r="D36" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>124</v>
-      </c>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
       <c r="F36" s="16" t="s">
         <v>96</v>
       </c>
@@ -2872,48 +2861,68 @@
       <c r="B37" s="15"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E37" s="16" t="s">
         <v>124</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>164</v>
+        <v>96</v>
       </c>
       <c r="G37" s="16" t="s">
         <v>7</v>
       </c>
       <c r="H37" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B38" s="15"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="17" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B38" s="30"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37" t="s">
+    <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B39" s="30"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="G38" s="37" t="s">
+      <c r="G39" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H38" s="38" t="s">
+      <c r="H39" s="38" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="21"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="23"/>
+    <row r="40" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="21"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add cs portinterfaces design
</commit_message>
<xml_diff>
--- a/Import/Application.xlsx
+++ b/Import/Application.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBC1F4E-445B-4FC5-A91B-EC244468CC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B16A16-F70A-4B17-BDA5-7F3FE81A6A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTypes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="173">
   <si>
     <t>TypeName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -421,10 +421,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ReturnValueType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>E_OK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -706,6 +702,22 @@
   </si>
   <si>
     <t>RefreshRequest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnumAppError</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AppErrors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_MotorAppError</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_MOTOR_APPERROR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1622,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A675E1F-9C03-4EE3-AE97-C268A8F23FBE}">
-  <dimension ref="B1:I71"/>
+  <dimension ref="B1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1720,7 +1732,7 @@
     </row>
     <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" s="37" t="s">
         <v>4</v>
@@ -1729,7 +1741,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1747,22 +1759,22 @@
         <v>1</v>
       </c>
       <c r="D11" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="F11" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="G11" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="H11" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="H11" s="28" t="s">
+      <c r="I11" s="29" t="s">
         <v>117</v>
-      </c>
-      <c r="I11" s="29" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.2">
@@ -1777,13 +1789,13 @@
     </row>
     <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E13" s="16">
         <v>0.1</v>
@@ -1798,18 +1810,18 @@
         <v>120</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D14" s="45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E14" s="37">
         <v>5.6250000000000001E-2</v>
@@ -1824,7 +1836,7 @@
         <v>240</v>
       </c>
       <c r="I14" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1860,7 +1872,7 @@
     </row>
     <row r="19" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B19" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>11</v>
@@ -1920,7 +1932,7 @@
     </row>
     <row r="25" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B25" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>11</v>
@@ -1960,13 +1972,13 @@
     </row>
     <row r="29" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B29" s="30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>11</v>
+        <v>169</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E29" s="38">
         <v>0</v>
@@ -1976,7 +1988,7 @@
       <c r="B30" s="30"/>
       <c r="C30" s="37"/>
       <c r="D30" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E30" s="38">
         <v>1</v>
@@ -1990,13 +2002,13 @@
     </row>
     <row r="32" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B32" s="30" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>11</v>
+        <v>169</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E32" s="38">
         <v>0</v>
@@ -2006,380 +2018,410 @@
       <c r="B33" s="30"/>
       <c r="C33" s="37"/>
       <c r="D33" s="42" t="s">
-        <v>103</v>
+        <v>172</v>
       </c>
       <c r="E33" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B34" s="30"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="E34" s="38">
-        <v>2</v>
-      </c>
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="20"/>
     </row>
     <row r="35" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="20"/>
+      <c r="B35" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="38">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B36" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="C36" s="37" t="s">
-        <v>11</v>
-      </c>
+      <c r="B36" s="30"/>
+      <c r="C36" s="37"/>
       <c r="D36" s="42" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="E36" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B37" s="30"/>
       <c r="C37" s="37"/>
       <c r="D37" s="42" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="E37" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B38" s="18"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="20"/>
+    </row>
+    <row r="39" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B39" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="E39" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B40" s="30"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" s="38">
         <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B38" s="30"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="E38" s="38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B39" s="18"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="20"/>
-    </row>
-    <row r="40" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B40" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="C40" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="E40" s="38">
-        <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B41" s="30"/>
       <c r="C41" s="37"/>
       <c r="D41" s="42" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E41" s="38">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B42" s="30"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="E42" s="38">
-        <v>2</v>
-      </c>
+      <c r="B42" s="18"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="20"/>
     </row>
     <row r="43" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B43" s="30"/>
-      <c r="C43" s="37"/>
+      <c r="B43" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="37" t="s">
+        <v>11</v>
+      </c>
       <c r="D43" s="42" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E43" s="38">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B44" s="30"/>
       <c r="C44" s="37"/>
       <c r="D44" s="42" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E44" s="38">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="20"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="E45" s="38">
+        <v>2</v>
+      </c>
     </row>
     <row r="46" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B46" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="C46" s="37" t="s">
-        <v>11</v>
-      </c>
+      <c r="B46" s="30"/>
+      <c r="C46" s="37"/>
       <c r="D46" s="42" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E46" s="38">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B47" s="30"/>
       <c r="C47" s="37"/>
       <c r="D47" s="42" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E47" s="38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B48" s="18"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="20"/>
+    </row>
+    <row r="49" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B49" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B50" s="30"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="E50" s="38">
         <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B48" s="30"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="42" t="s">
-        <v>140</v>
-      </c>
-      <c r="E48" s="38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="20"/>
-    </row>
-    <row r="50" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B50" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="C50" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="E50" s="38">
-        <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B51" s="30"/>
       <c r="C51" s="37"/>
       <c r="D51" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="E51" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B52" s="18"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="20"/>
+    </row>
+    <row r="53" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B53" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C53" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E53" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B54" s="30"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="E54" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B55" s="30"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="E51" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B52" s="30"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="E52" s="38">
+      <c r="E55" s="38">
         <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B53" s="30"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="42" t="s">
-        <v>145</v>
-      </c>
-      <c r="E53" s="38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B54" s="18"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="20"/>
-    </row>
-    <row r="55" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B55" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="C55" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="42" t="s">
-        <v>148</v>
-      </c>
-      <c r="E55" s="38">
-        <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B56" s="30"/>
       <c r="C56" s="37"/>
       <c r="D56" s="42" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E56" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B57" s="18"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="20"/>
+    </row>
+    <row r="58" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B58" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B59" s="30"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="E59" s="38">
         <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B57" s="30"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="42" t="s">
-        <v>150</v>
-      </c>
-      <c r="E57" s="38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B58" s="18"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="20"/>
-    </row>
-    <row r="59" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B59" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C59" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D59" s="42" t="s">
-        <v>153</v>
-      </c>
-      <c r="E59" s="38">
-        <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B60" s="30"/>
       <c r="C60" s="37"/>
       <c r="D60" s="42" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E60" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B61" s="18"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="20"/>
+    </row>
+    <row r="62" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B62" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C62" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="E62" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B63" s="30"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E63" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="7"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="9"/>
-    </row>
-    <row r="62" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D62" s="11"/>
-    </row>
-    <row r="63" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="27" t="s">
+    <row r="64" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="7"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="9"/>
+    </row>
+    <row r="65" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D65" s="11"/>
+    </row>
+    <row r="66" spans="2:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C63" s="28" t="s">
+      <c r="C66" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D63" s="28" t="s">
+      <c r="D66" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E63" s="29" t="s">
+      <c r="E66" s="29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B64" s="1"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="3"/>
-    </row>
-    <row r="65" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B65" s="15" t="s">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B67" s="1"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B68" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C68" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="D68" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="17" t="s">
+      <c r="E68" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B66" s="15"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16" t="s">
+    <row r="69" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B69" s="15"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="17" t="s">
+      <c r="E69" s="17" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B67" s="15"/>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E67" s="17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B68" s="18"/>
-      <c r="C68" s="19"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="20"/>
-    </row>
-    <row r="69" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B69" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C69" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D69" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E69" s="17" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="70" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B70" s="15"/>
       <c r="C70" s="16"/>
       <c r="D70" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B71" s="18"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="20"/>
+    </row>
+    <row r="72" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B72" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B73" s="15"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E70" s="17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="7"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="9"/>
+      <c r="E73" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="7"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2392,17 +2434,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA44D0C-18C8-469C-9219-A37B0C48C99E}">
   <dimension ref="B2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.125" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="16.25" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="3" max="4" width="16.25" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="17.25" customWidth="1"/>
     <col min="7" max="7" width="22.75" customWidth="1"/>
     <col min="8" max="8" width="26.5" customWidth="1"/>
@@ -2552,16 +2593,16 @@
         <v>1</v>
       </c>
       <c r="D18" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" s="28" t="s">
         <v>92</v>
-      </c>
-      <c r="E18" s="28" t="s">
-        <v>98</v>
       </c>
       <c r="F18" s="28" t="s">
         <v>93</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H18" s="29" t="s">
         <v>84</v>
@@ -2584,16 +2625,16 @@
         <v>91</v>
       </c>
       <c r="D20" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>94</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>124</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>36</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H20" s="17" t="s">
         <v>97</v>
@@ -2602,17 +2643,15 @@
     <row r="21" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="16"/>
+      <c r="E21" s="16" t="s">
         <v>95</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>124</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>36</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H21" s="17" t="s">
         <v>97</v>
@@ -2621,20 +2660,18 @@
     <row r="22" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
-      <c r="D22" s="16" t="s">
-        <v>101</v>
-      </c>
+      <c r="D22" s="16"/>
       <c r="E22" s="16" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15" x14ac:dyDescent="0.2">
@@ -2643,13 +2680,13 @@
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="15" x14ac:dyDescent="0.2">
@@ -2658,13 +2695,13 @@
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>107</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15" x14ac:dyDescent="0.2">
@@ -2673,13 +2710,13 @@
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15" x14ac:dyDescent="0.2">
@@ -2688,13 +2725,13 @@
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="15" x14ac:dyDescent="0.2">
@@ -2703,10 +2740,10 @@
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>97</v>
@@ -2715,11 +2752,9 @@
     <row r="28" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B28" s="15"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="16" t="s">
-        <v>169</v>
-      </c>
+      <c r="D28" s="16"/>
       <c r="E28" s="16" t="s">
-        <v>124</v>
+        <v>168</v>
       </c>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
@@ -2736,25 +2771,25 @@
     </row>
     <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B30" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>91</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="15" x14ac:dyDescent="0.2">
@@ -2766,7 +2801,7 @@
         <v>96</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H31" s="17" t="s">
         <v>97</v>
@@ -2775,11 +2810,9 @@
     <row r="32" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
-      <c r="D32" s="16" t="s">
-        <v>155</v>
-      </c>
+      <c r="D32" s="16"/>
       <c r="E32" s="16" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>96</v>
@@ -2794,20 +2827,18 @@
     <row r="33" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B33" s="15"/>
       <c r="C33" s="16"/>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="16"/>
+      <c r="E33" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F33" s="16" t="s">
         <v>156</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>157</v>
       </c>
       <c r="G33" s="16" t="s">
         <v>2</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.2">
@@ -2821,25 +2852,25 @@
     </row>
     <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B35" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>91</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>7</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.2">
@@ -2860,11 +2891,9 @@
     <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B37" s="15"/>
       <c r="C37" s="16"/>
-      <c r="D37" s="16" t="s">
-        <v>162</v>
-      </c>
+      <c r="D37" s="16"/>
       <c r="E37" s="16" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>96</v>
@@ -2879,20 +2908,18 @@
     <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B38" s="15"/>
       <c r="C38" s="16"/>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="16"/>
+      <c r="E38" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="F38" s="16" t="s">
         <v>163</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>164</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>7</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.2">
@@ -2901,7 +2928,7 @@
       <c r="D39" s="37"/>
       <c r="E39" s="37"/>
       <c r="F39" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G39" s="37" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
finish cs interface support implementation
</commit_message>
<xml_diff>
--- a/Import/Application.xlsx
+++ b/Import/Application.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B16A16-F70A-4B17-BDA5-7F3FE81A6A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEBC51E-23E4-4FFA-9B23-4815B4ACBDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTypes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="177">
   <si>
     <t>TypeName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -718,6 +718,22 @@
   </si>
   <si>
     <t>E_MOTOR_APPERROR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_CockpitService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_MotorCtrService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_DoorLockService</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1636,7 +1652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A675E1F-9C03-4EE3-AE97-C268A8F23FBE}">
   <dimension ref="B1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -2435,7 +2451,7 @@
   <dimension ref="B2:H40"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2955,10 +2971,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A1755F-5E81-4222-BC5B-9CFC616875A8}">
-  <dimension ref="B1:J20"/>
+  <dimension ref="B1:J23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3118,53 +3134,55 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="4"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="15" t="s">
+    <row r="9" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B9" s="15"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B11" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C11" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="17"/>
-    </row>
-    <row r="11" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="15"/>
-      <c r="C11" s="32"/>
       <c r="D11" s="16" t="s">
         <v>61</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F11" s="16"/>
-      <c r="G11" s="16" t="s">
-        <v>75</v>
-      </c>
+      <c r="G11" s="16"/>
       <c r="H11" s="16" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
@@ -3173,88 +3191,86 @@
       <c r="B12" s="15"/>
       <c r="C12" s="32"/>
       <c r="D12" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="17"/>
+    </row>
+    <row r="13" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B13" s="15"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E13" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F13" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16" t="s">
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J13" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="4"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
-    </row>
     <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>67</v>
-      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="16" t="s">
         <v>62</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="15"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B16" s="15"/>
-      <c r="C16" s="32"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>67</v>
+      </c>
       <c r="D16" s="16" t="s">
         <v>62</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>85</v>
@@ -3264,78 +3280,140 @@
       <c r="I16" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="4"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>65</v>
-      </c>
+      <c r="J16" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B17" s="15"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="B18" s="15"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="16" t="s">
         <v>62</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="J18" s="41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B20" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J20" s="17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="30"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="37" t="s">
+    <row r="21" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B21" s="30"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E21" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F21" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37" t="s">
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="J19" s="38"/>
-    </row>
-    <row r="20" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="9"/>
+      <c r="J21" s="38"/>
+    </row>
+    <row r="22" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B22" s="15"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="J22" s="17"/>
+    </row>
+    <row r="23" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>